<commit_message>
Grid Test Stones Added
</commit_message>
<xml_diff>
--- a/Assets/Resources/PaperMissionTracker.xlsx
+++ b/Assets/Resources/PaperMissionTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connorcolombo/Documents/PKBACK/GitHub/cuberover-simulator/Assets/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1762BFB4-CF0F-DB42-AC24-9CE9C10EA838}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3727ED9-B8CC-284D-A3E3-2D21023B07D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20660" xr2:uid="{9DC019AC-4F4E-3F4C-BAEF-F7D1E1ACF78C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20620" xr2:uid="{9DC019AC-4F4E-3F4C-BAEF-F7D1E1ACF78C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -554,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E5BD28-A13F-6248-8C78-F6F357A35069}">
   <dimension ref="A1:AG892"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="AG12" sqref="AG12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Added Slippage Simulation, Deployment, Diagnostics, and did some Code Refactoring (Clean up)
Undeploy still needs some work (can reset quaternion but not teleport).
Pseudosensors need to be added.
Heading Displacement is broken (probably due to bounding with Atan2)
</commit_message>
<xml_diff>
--- a/Assets/Resources/PaperMissionTracker.xlsx
+++ b/Assets/Resources/PaperMissionTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connorcolombo/Documents/PKBACK/GitHub/cuberover-simulator/Assets/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3727ED9-B8CC-284D-A3E3-2D21023B07D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF99951-59EF-DE4C-957C-28DF14848249}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20620" xr2:uid="{9DC019AC-4F4E-3F4C-BAEF-F7D1E1ACF78C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20600" xr2:uid="{9DC019AC-4F4E-3F4C-BAEF-F7D1E1ACF78C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -555,7 +555,7 @@
   <dimension ref="A1:AG892"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -567,6 +567,7 @@
     <col min="15" max="15" width="0.83203125" style="6" customWidth="1"/>
     <col min="21" max="21" width="0.83203125" style="6" customWidth="1"/>
     <col min="27" max="27" width="0.83203125" style="6" customWidth="1"/>
+    <col min="29" max="29" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -2676,10 +2677,7 @@
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="X23" s="7" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
+      <c r="X23" s="7"/>
       <c r="Y23" s="7" t="str">
         <f t="shared" si="16"/>
         <v/>
@@ -6458,9 +6456,9 @@
         <f t="array" aca="1" ref="AC61" ca="1">IFERROR(INDIRECT(_xlfn.SWITCH(MOD((ROW(AC61)-ROW(AC$5)),3),0,CHAR(COLUMN(K61)+64),1,CHAR(COLUMN(Q61)+64),2,CHAR(COLUMN(W61)+64))&amp;(ROW(K$5)+INT((ROW(AC61)-ROW(AC$5))/3))),"")</f>
         <v/>
       </c>
-      <c r="AD61" s="2" t="str" cm="1">
+      <c r="AD61" s="2" cm="1">
         <f t="array" aca="1" ref="AD61" ca="1">IFERROR(ROUND(INDIRECT(_xlfn.SWITCH(MOD((ROW(AD61)-ROW(AD$5)),3),0,CHAR(COLUMN(L61)+64),1,CHAR(COLUMN(R61)+64),2,CHAR(COLUMN(X61)+64))&amp;(ROW(L$5)+INT((ROW(AD61)-ROW(AD$5))/3))),0),"")</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="AE61" s="2"/>
       <c r="AF61" s="2" t="str" cm="1">

</xml_diff>